<commit_message>
Versão entregue no moodle
</commit_message>
<xml_diff>
--- a/Documentação/Backlog Projeto Individual.xlsx
+++ b/Documentação/Backlog Projeto Individual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paesl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paesl\sptech\GitHub\Projeto-Pessoal\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD48E5A3-0735-4F47-8B1A-69D3EB77763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2835FC9-D4CA-4993-870A-8F03DF0BE9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>Requisito</t>
   </si>
@@ -103,13 +103,16 @@
   </si>
   <si>
     <t>5.11 Tela de Regra de Três</t>
+  </si>
+  <si>
+    <t>6.0 Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +129,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -180,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1281,6 +1292,50 @@
         <a:xfrm>
           <a:off x="1950840" y="38833426"/>
           <a:ext cx="2954536" cy="1142279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1337612</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2992079</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2076450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagem 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A1CDA2-9DD0-30E6-FCA2-382CB70345DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1947212" y="39976426"/>
+          <a:ext cx="2997492" cy="2076449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1609,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,12 +1886,26 @@
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="21" spans="2:5" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>